<commit_message>
use separate compare function for comparing inhoud
</commit_message>
<xml_diff>
--- a/static/hb6000.xlsx
+++ b/static/hb6000.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelte\WebstormProjects\bodyblock-conversion\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeltedirks/WebstormProjects/bodyblock-conversion/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE02526-BCAB-4260-BC1B-3CF486B4CF9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CFEF8A-82AB-824C-8BCF-1D7BA508C47A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9000" yWindow="7245" windowWidth="16860" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2200" yWindow="2560" windowWidth="22900" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="06020" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>P302</t>
   </si>
@@ -45,9 +45,6 @@
     <t>niet verwijderen</t>
   </si>
   <si>
-    <t>Label</t>
-  </si>
-  <si>
     <t>omschrijving</t>
   </si>
   <si>
@@ -67,6 +64,21 @@
   </si>
   <si>
     <t>Gezinssamenstelling</t>
+  </si>
+  <si>
+    <t>Eigen risico</t>
+  </si>
+  <si>
+    <t>€ 10043  10044</t>
+  </si>
+  <si>
+    <t>rechts</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>10631 10632 10630          10633</t>
   </si>
 </sst>
 </file>
@@ -102,8 +114,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -384,49 +399,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="8" width="18" customWidth="1"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="7" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="69" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
       </c>
       <c r="B2">
         <v>10694</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -434,7 +453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>10046</v>
       </c>
@@ -445,7 +464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>10050</v>
       </c>
@@ -456,9 +475,86 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>10043</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>10044</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>10631</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>10632</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>10630</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>10633</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
uses i o and a arguments. use --help to see what they do
</commit_message>
<xml_diff>
--- a/static/hb6000.xlsx
+++ b/static/hb6000.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeltedirks/WebstormProjects/bodyblock-conversion/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CD4568-49F1-E34B-95DE-F3CDA4C5F51A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D1EAC4-3D4B-0E4A-B7D8-DC3E2C585C4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="2560" windowWidth="22900" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="06020b" sheetId="1" r:id="rId1"/>
+    <sheet name="blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,32 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>P302</t>
-  </si>
-  <si>
-    <t>omschrijving</t>
-  </si>
-  <si>
-    <t>inhoud</t>
-  </si>
-  <si>
-    <t>weergave</t>
-  </si>
-  <si>
-    <t>uitlijnen</t>
-  </si>
-  <si>
-    <t>regel verwijderen</t>
-  </si>
-  <si>
-    <t>regel template</t>
-  </si>
-  <si>
-    <t>Gezinssamenstelling</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -369,10 +344,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -384,36 +359,14 @@
     <col min="8" max="8" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="69" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>10694</v>
-      </c>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>